<commit_message>
Changes of Amazon Project
</commit_message>
<xml_diff>
--- a/DataForTest/AnujaDDT.xlsx
+++ b/DataForTest/AnujaDDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganesh\eclipse-workspace\AmazonProject1\DataForTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202DAA55-35DA-45E9-8258-6D97F14031F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A8A415-0E8D-4F44-B6C4-0D5BEDF33D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>